<commit_message>
Added page to plan
</commit_message>
<xml_diff>
--- a/Plan.xlsx
+++ b/Plan.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Documents\Coding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6DFE5D-484E-499B-B175-6D9935556CF9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEC0811-8E99-43A6-9247-80DF2081EE9E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{36830CD4-5D0D-4EE0-AD98-5F61D0A27FB6}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{36830CD4-5D0D-4EE0-AD98-5F61D0A27FB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="45">
   <si>
     <t>Phase 2 - Create Model</t>
   </si>
@@ -100,6 +101,72 @@
   </si>
   <si>
     <t>Determine Data Source</t>
+  </si>
+  <si>
+    <t>- if not or it’s deemed too impractical, need to look into developing our own live charting or regularly updated charts</t>
+  </si>
+  <si>
+    <t>- charting: can etoro take an overlay? Eg we produce a txt file, upload it and it produces a series of points on the chart that are the prediction points</t>
+  </si>
+  <si>
+    <t>- our own time and availability to trade: we both have full time jobs, lives etc, how will this factor in - we need to produce an output that we can use to trade given our time availabilities</t>
+  </si>
+  <si>
+    <t>- keep output simple and decision making complex Eg model simply advises with its predictions we then do the decision making</t>
+  </si>
+  <si>
+    <t>BUY/SELL INDICATORS</t>
+  </si>
+  <si>
+    <t>Accuracy so far this month</t>
+  </si>
+  <si>
+    <t>Cumulative value accuracy</t>
+  </si>
+  <si>
+    <t>Averaged value accuract</t>
+  </si>
+  <si>
+    <t>Cumulative delta accuracy</t>
+  </si>
+  <si>
+    <t>Averaged delta accuracy</t>
+  </si>
+  <si>
+    <t>Averaged st. dev</t>
+  </si>
+  <si>
+    <t>no. points in boxplot</t>
+  </si>
+  <si>
+    <t>no. points in box</t>
+  </si>
+  <si>
+    <t>no. correct directions</t>
+  </si>
+  <si>
+    <t>Local Accuracy</t>
+  </si>
+  <si>
+    <t>Montly accuracy indicators for local dataset, with focus on delta values (not absolute error)</t>
+  </si>
+  <si>
+    <t>Averaged value accuracy gradient</t>
+  </si>
+  <si>
+    <t>Buy/Sell deltaT</t>
+  </si>
+  <si>
+    <t>Absolute value gradient</t>
+  </si>
+  <si>
+    <t>Potential gain/loss</t>
+  </si>
+  <si>
+    <t>Overnight?</t>
+  </si>
+  <si>
+    <t>Delta t length</t>
   </si>
 </sst>
 </file>
@@ -163,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -172,6 +239,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,7 +556,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0BC3E5CD-980A-4F59-835A-ACF3EA83A590}">
   <dimension ref="A1:W27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N27" sqref="N27"/>
     </sheetView>
   </sheetViews>
@@ -774,4 +842,135 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E01E07AC-7931-48B7-AE21-C52B9D82EC58}">
+  <dimension ref="A1:A24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>